<commit_message>
duplicate rollno exception done
</commit_message>
<xml_diff>
--- a/uploads/test_file.xlsx
+++ b/uploads/test_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096872C1-DCF1-4FA7-90B0-337D12228659}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7EFF39-F1B5-4601-AA5F-11C881EE10B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{70E6F6CC-AFD8-4038-9A93-B7DFE2A78E7D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>ATKALE PRAGATI PRAMOD</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>WANGADARE KOMAL RAJENDRA</t>
+  </si>
+  <si>
+    <t>WANGADARE KOM RAJENDRA</t>
   </si>
 </sst>
 </file>
@@ -712,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD65262-F4BC-4879-AC53-D0B85E76AFA4}">
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" zoomScale="136" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1620,65 +1623,78 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C65"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C65" s="22">
+        <v>2018032500246990</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C66"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C67"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C68"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C71"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C72" s="20"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="20"/>
-      <c r="C73"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C71" s="20"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="20"/>
+      <c r="C72"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C73" s="20"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C74" s="20"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B75" s="7"/>
       <c r="C75" s="20"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B76" s="7"/>
       <c r="C76" s="20"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B77" s="7"/>
       <c r="C77" s="20"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="4"/>
       <c r="B78" s="7"/>
       <c r="C78" s="20"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="4"/>
-      <c r="B79" s="7"/>
+    <row r="79" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="5"/>
+      <c r="B79" s="17"/>
       <c r="C79" s="20"/>
     </row>
-    <row r="80" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
-      <c r="B80" s="17"/>
+      <c r="B80" s="18"/>
       <c r="C80" s="20"/>
     </row>
-    <row r="81" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
-      <c r="B81" s="18"/>
+      <c r="B81" s="7"/>
       <c r="C81" s="20"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -1687,8 +1703,8 @@
       <c r="C82" s="20"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="5"/>
-      <c r="B83" s="7"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="19"/>
       <c r="C83" s="20"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -1708,7 +1724,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
-      <c r="B87" s="19"/>
+      <c r="B87" s="7"/>
       <c r="C87" s="20"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -6270,11 +6286,6 @@
       <c r="A999" s="4"/>
       <c r="B999" s="7"/>
       <c r="C999" s="20"/>
-    </row>
-    <row r="1000" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1000" s="4"/>
-      <c r="B1000" s="7"/>
-      <c r="C1000" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
admin report done div wise and dept wise year and div done
</commit_message>
<xml_diff>
--- a/uploads/test_file.xlsx
+++ b/uploads/test_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948268B3-7C65-4D9F-BC1E-0516540DC8EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECB2BFE-5291-4089-867B-AABF0AC01476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{70E6F6CC-AFD8-4038-9A93-B7DFE2A78E7D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
   <si>
     <t>ATKALE PRAGATI PRAMOD</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>WANGADARE KOMAL RAJENDRA</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
   </si>
 </sst>
 </file>
@@ -712,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD65262-F4BC-4879-AC53-D0B85E76AFA4}">
-  <dimension ref="A1:D997"/>
+  <dimension ref="A1:E997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="136" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,7 +736,7 @@
     <col min="3" max="3" width="30.109375" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -734,11 +746,14 @@
       <c r="C1" s="22">
         <v>2019032500202240</v>
       </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -748,11 +763,14 @@
       <c r="C2" s="22">
         <v>2019032500202450</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -762,11 +780,14 @@
       <c r="C3" s="22">
         <v>2019032500202420</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -776,11 +797,14 @@
       <c r="C4" s="22">
         <v>2019032500202310</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -790,11 +814,14 @@
       <c r="C5" s="22">
         <v>2019032500202110</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -804,11 +831,14 @@
       <c r="C6" s="22">
         <v>2019032500202430</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -818,11 +848,14 @@
       <c r="C7" s="22">
         <v>2019032500202380</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -832,11 +865,14 @@
       <c r="C8" s="22">
         <v>2019032500202340</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -846,11 +882,14 @@
       <c r="C9" s="22">
         <v>2019032500202660</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -860,11 +899,14 @@
       <c r="C10" s="22">
         <v>2019032500202260</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -874,11 +916,14 @@
       <c r="C11" s="22">
         <v>2019032500202570</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -888,11 +933,14 @@
       <c r="C12" s="22">
         <v>2019032500202370</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -902,11 +950,14 @@
       <c r="C13" s="22">
         <v>2019032500202080</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -916,11 +967,14 @@
       <c r="C14" s="22">
         <v>2019032500202630</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -930,11 +984,14 @@
       <c r="C15" s="22">
         <v>2019032500202410</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -944,11 +1001,14 @@
       <c r="C16" s="22">
         <v>2019032500202320</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -958,11 +1018,14 @@
       <c r="C17" s="22">
         <v>2019032500202220</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -972,11 +1035,14 @@
       <c r="C18" s="22">
         <v>2019032500202690</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -986,11 +1052,14 @@
       <c r="C19" s="22">
         <v>2019032500202200</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1000,11 +1069,14 @@
       <c r="C20" s="22">
         <v>2019032500202390</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1014,11 +1086,14 @@
       <c r="C21" s="22">
         <v>2019032500202710</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1028,11 +1103,14 @@
       <c r="C22" s="22">
         <v>2019032500202680</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -1042,11 +1120,14 @@
       <c r="C23" s="22">
         <v>2019032500202290</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -1056,11 +1137,14 @@
       <c r="C24" s="22">
         <v>2019032500202360</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -1070,11 +1154,14 @@
       <c r="C25" s="22">
         <v>2019032500202300</v>
       </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -1084,11 +1171,14 @@
       <c r="C26" s="22">
         <v>2019032500202140</v>
       </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -1098,11 +1188,14 @@
       <c r="C27" s="22">
         <v>2019032500202600</v>
       </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>28</v>
       </c>
@@ -1112,11 +1205,14 @@
       <c r="C28" s="22">
         <v>2019032500202130</v>
       </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>29</v>
       </c>
@@ -1126,11 +1222,14 @@
       <c r="C29" s="22">
         <v>2019032500202150</v>
       </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>30</v>
       </c>
@@ -1140,11 +1239,14 @@
       <c r="C30" s="22">
         <v>2019032500202670</v>
       </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>31</v>
       </c>
@@ -1154,11 +1256,14 @@
       <c r="C31" s="22">
         <v>2019032500202550</v>
       </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>32</v>
       </c>
@@ -1168,11 +1273,14 @@
       <c r="C32" s="22">
         <v>2019032500202230</v>
       </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>33</v>
       </c>
@@ -1182,11 +1290,14 @@
       <c r="C33" s="22">
         <v>2019032500202460</v>
       </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>34</v>
       </c>
@@ -1196,11 +1307,14 @@
       <c r="C34" s="22">
         <v>2019032500202090</v>
       </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>35</v>
       </c>
@@ -1210,11 +1324,14 @@
       <c r="C35" s="22">
         <v>2019032500202210</v>
       </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -1224,11 +1341,14 @@
       <c r="C36" s="22">
         <v>2019032500202350</v>
       </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>37</v>
       </c>
@@ -1238,11 +1358,14 @@
       <c r="C37" s="22">
         <v>2019032500202540</v>
       </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>38</v>
       </c>
@@ -1252,11 +1375,14 @@
       <c r="C38" s="22">
         <v>2019032500202120</v>
       </c>
-      <c r="D38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>39</v>
       </c>
@@ -1266,11 +1392,14 @@
       <c r="C39" s="22">
         <v>2019032500202170</v>
       </c>
-      <c r="D39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -1280,11 +1409,14 @@
       <c r="C40" s="22">
         <v>2019032500202470</v>
       </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -1294,11 +1426,14 @@
       <c r="C41" s="22">
         <v>2019032500202700</v>
       </c>
-      <c r="D41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>42</v>
       </c>
@@ -1308,11 +1443,14 @@
       <c r="C42" s="22">
         <v>2019032500202730</v>
       </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -1322,11 +1460,14 @@
       <c r="C43" s="22">
         <v>2019032500202560</v>
       </c>
-      <c r="D43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -1336,11 +1477,14 @@
       <c r="C44" s="22">
         <v>2019032500202640</v>
       </c>
-      <c r="D44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45</v>
       </c>
@@ -1350,11 +1494,14 @@
       <c r="C45" s="22">
         <v>2019032500202180</v>
       </c>
-      <c r="D45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -1364,11 +1511,14 @@
       <c r="C46" s="22">
         <v>2019032500202400</v>
       </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -1378,11 +1528,14 @@
       <c r="C47" s="22">
         <v>2019032500202590</v>
       </c>
-      <c r="D47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>48</v>
       </c>
@@ -1392,11 +1545,14 @@
       <c r="C48" s="22">
         <v>2019032500202440</v>
       </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>49</v>
       </c>
@@ -1406,11 +1562,14 @@
       <c r="C49" s="22">
         <v>2019032500202270</v>
       </c>
-      <c r="D49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>50</v>
       </c>
@@ -1420,11 +1579,14 @@
       <c r="C50" s="22">
         <v>2019032500202190</v>
       </c>
-      <c r="D50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>51</v>
       </c>
@@ -1434,11 +1596,14 @@
       <c r="C51" s="22">
         <v>2019032500202720</v>
       </c>
-      <c r="D51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>52</v>
       </c>
@@ -1448,11 +1613,14 @@
       <c r="C52" s="22">
         <v>2019032500202330</v>
       </c>
-      <c r="D52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>53</v>
       </c>
@@ -1462,11 +1630,14 @@
       <c r="C53" s="22">
         <v>2019032500202530</v>
       </c>
-      <c r="D53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>54</v>
       </c>
@@ -1476,11 +1647,14 @@
       <c r="C54" s="22">
         <v>2019032500202100</v>
       </c>
-      <c r="D54">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>55</v>
       </c>
@@ -1490,11 +1664,14 @@
       <c r="C55" s="22">
         <v>2019032500202480</v>
       </c>
-      <c r="D55">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>56</v>
       </c>
@@ -1504,11 +1681,14 @@
       <c r="C56" s="22">
         <v>2019032500202580</v>
       </c>
-      <c r="D56">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>67</v>
+      </c>
+      <c r="E56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>57</v>
       </c>
@@ -1518,11 +1698,14 @@
       <c r="C57" s="22">
         <v>2019032500202250</v>
       </c>
-      <c r="D57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>67</v>
+      </c>
+      <c r="E57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>58</v>
       </c>
@@ -1532,11 +1715,14 @@
       <c r="C58" s="22">
         <v>2019032500202610</v>
       </c>
-      <c r="D58">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>59</v>
       </c>
@@ -1546,11 +1732,14 @@
       <c r="C59" s="22">
         <v>2018032500246970</v>
       </c>
-      <c r="D59">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>67</v>
+      </c>
+      <c r="E59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>60</v>
       </c>
@@ -1560,11 +1749,14 @@
       <c r="C60" s="22">
         <v>2016032500221080</v>
       </c>
-      <c r="D60">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>61</v>
       </c>
@@ -1574,11 +1766,14 @@
       <c r="C61" s="22">
         <v>2018032500247010</v>
       </c>
-      <c r="D61">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>62</v>
       </c>
@@ -1588,11 +1783,14 @@
       <c r="C62" s="22">
         <v>2018032500246960</v>
       </c>
-      <c r="D62">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>63</v>
       </c>
@@ -1602,11 +1800,14 @@
       <c r="C63" s="22">
         <v>2016032500220230</v>
       </c>
-      <c r="D63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>64</v>
       </c>
@@ -1616,8 +1817,11 @@
       <c r="C64" s="22">
         <v>2018032500246990</v>
       </c>
-      <c r="D64">
-        <v>3</v>
+      <c r="D64" t="s">
+        <v>67</v>
+      </c>
+      <c r="E64" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>